<commit_message>
Final Sportify India Project
</commit_message>
<xml_diff>
--- a/Documents/Sportify India UML Diagram & DB Schema3.xlsx
+++ b/Documents/Sportify India UML Diagram & DB Schema3.xlsx
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:V135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,17 +1061,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="3:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:16" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="3:16" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="3:16" ht="14.55" x14ac:dyDescent="0.35"/>
     <row r="27" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D27" s="17" t="s">
         <v>13</v>
@@ -1092,7 +1091,7 @@
       <c r="H28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="3:16" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D29" s="7" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="3:16" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D30" s="7" t="s">
         <v>46</v>
       </c>
@@ -1120,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="3:16" ht="14.55" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D31" s="7" t="s">
         <v>47</v>
       </c>
@@ -1136,8 +1135,7 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="3:16" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="4:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>

</xml_diff>